<commit_message>
Added backward compatibility for data collected in TubulenceDatalogger v1. This change eliminates the need for payloadSpin v1.
</commit_message>
<xml_diff>
--- a/data/NovTwoBalloon/Nov_16_Two_Balloon_IMU_Data.xlsx
+++ b/data/NovTwoBalloon/Nov_16_Two_Balloon_IMU_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\MSGC\Payload Sway n Spin Reduction\IMU Data\NovTwoBalloon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\MSGC\IMU\Processing\payloadSpin\data\NovTwoBalloon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -295,10 +295,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -352,69 +352,75 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$20</c:f>
+              <c:f>Sheet1!$B$3:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3484</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6879</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7143</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6968</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5803</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6761</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5864</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4503</c:v>
+                  <c:v>615</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4965</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7251</c:v>
+                  <c:v>488</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5897</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7291</c:v>
+                  <c:v>996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6941</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8642</c:v>
+                  <c:v>948</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7034</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7307</c:v>
+                  <c:v>1199</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4457</c:v>
+                  <c:v>681</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1450</c:v>
+                  <c:v>991</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,10 +468,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -519,69 +525,75 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$20</c:f>
+              <c:f>Sheet1!$E$3:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5579</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7169</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6468</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6466</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7030</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6124</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5171</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6254</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5147</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6500</c:v>
+                  <c:v>577</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6499</c:v>
+                  <c:v>1347</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7203</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4688</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8045</c:v>
+                  <c:v>604</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7948</c:v>
+                  <c:v>859</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5353</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6345</c:v>
+                  <c:v>748</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2263</c:v>
+                  <c:v>781</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,10 +639,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -684,69 +696,75 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$20</c:f>
+              <c:f>Sheet1!$H$3:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5226</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6539</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7080</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6962</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5745</c:v>
+                  <c:v>331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7763</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7120</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3992</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5317</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5505</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7639</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7944</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8268</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7053</c:v>
+                  <c:v>633</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7351</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6175</c:v>
+                  <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7826</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3675</c:v>
+                  <c:v>759</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -794,10 +812,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -851,60 +869,63 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$20</c:f>
+              <c:f>Sheet1!$K$3:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5248</c:v>
+                  <c:v>333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5573</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7098</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5180</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5872</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5017</c:v>
+                  <c:v>571</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5459</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6959</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7265</c:v>
+                  <c:v>383</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6836</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5485</c:v>
+                  <c:v>936</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5644</c:v>
+                  <c:v>955</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5409</c:v>
+                  <c:v>1101</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4299</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3828</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,10 +971,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1007,60 +1028,63 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$3:$N$20</c:f>
+              <c:f>Sheet1!$N$3:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>4144</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4791</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4263</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5010</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7905</c:v>
+                  <c:v>757</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8495</c:v>
+                  <c:v>492</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7024</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5302</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5305</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8144</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6364</c:v>
+                  <c:v>786</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5694</c:v>
+                  <c:v>868</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6043</c:v>
+                  <c:v>908</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4748</c:v>
+                  <c:v>934</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4701</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1184,7 +1208,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1498,10 +1522,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1555,21 +1579,24 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$20</c:f>
+              <c:f>Sheet1!$C$3:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>102</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1578,31 +1605,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1611,12 +1638,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1662,10 +1692,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1719,27 +1749,30 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$20</c:f>
+              <c:f>Sheet1!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1751,13 +1784,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1781,6 +1814,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1826,10 +1862,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1883,69 +1919,75 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$20</c:f>
+              <c:f>Sheet1!$I$3:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>183</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>154</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>116</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>109</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>114</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>74</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>55</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>64</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>116</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,10 +2030,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -2045,60 +2087,63 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$20</c:f>
+              <c:f>Sheet1!$L$3:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>131</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>190</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>204</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>253</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>198</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>68</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>58</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>69</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,10 +2186,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -2198,39 +2243,42 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$3:$O$20</c:f>
+              <c:f>Sheet1!$O$3:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>194</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>129</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>247</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2239,7 +2287,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -2370,7 +2418,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2683,10 +2731,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -2740,57 +2788,60 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$20</c:f>
+              <c:f>Sheet1!$D$3:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2802,6 +2853,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2847,10 +2901,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -2904,42 +2958,45 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$20</c:f>
+              <c:f>Sheet1!$G$3:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>82</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2948,10 +3005,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -2963,9 +3020,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3011,10 +3071,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -3068,21 +3128,24 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$20</c:f>
+              <c:f>Sheet1!$J$3:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>94</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3091,28 +3154,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3121,7 +3184,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -3130,6 +3193,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3173,10 +3239,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -3230,36 +3296,39 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$20</c:f>
+              <c:f>Sheet1!$M$3:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>278</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>306</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>228</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>276</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3326,10 +3395,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
+              <c:f>Sheet1!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -3383,39 +3452,42 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$P$20</c:f>
+              <c:f>Sheet1!$P$3:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>245</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>232</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>216</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3555,7 +3627,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5837,29 +5909,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE28" sqref="AE28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5939,49 +5996,49 @@
         <v>5000</v>
       </c>
       <c r="B3">
-        <v>3484</v>
+        <v>235</v>
       </c>
       <c r="C3">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E3">
-        <v>5579</v>
+        <v>159</v>
       </c>
       <c r="F3">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="H3">
-        <v>5226</v>
+        <v>104</v>
       </c>
       <c r="I3">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>5248</v>
+        <v>333</v>
       </c>
       <c r="L3">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>278</v>
+        <v>50</v>
       </c>
       <c r="N3">
-        <v>4144</v>
+        <v>7</v>
       </c>
       <c r="O3">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
@@ -5989,49 +6046,49 @@
         <v>10000</v>
       </c>
       <c r="B4">
-        <v>6879</v>
+        <v>155</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>7169</v>
+        <v>152</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>6539</v>
+        <v>154</v>
       </c>
       <c r="I4">
-        <v>171</v>
+        <v>15</v>
       </c>
       <c r="J4">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>5573</v>
+        <v>640</v>
       </c>
       <c r="L4">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>4791</v>
+        <v>66</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -6039,7 +6096,7 @@
         <v>15000</v>
       </c>
       <c r="B5">
-        <v>7143</v>
+        <v>66</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -6048,40 +6105,40 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6468</v>
+        <v>105</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
       </c>
       <c r="G5" s="11">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H5" s="11">
-        <v>7080</v>
+        <v>218</v>
       </c>
       <c r="I5" s="11">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="J5" s="11">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>7098</v>
+        <v>608</v>
       </c>
       <c r="L5">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>306</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>4263</v>
+        <v>65</v>
       </c>
       <c r="O5">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -6089,49 +6146,49 @@
         <v>20000</v>
       </c>
       <c r="B6">
-        <v>6968</v>
+        <v>317</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>6466</v>
+        <v>480</v>
       </c>
       <c r="F6" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G6" s="11">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H6" s="11">
-        <v>6962</v>
+        <v>173</v>
       </c>
       <c r="I6" s="11">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J6" s="11">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>5180</v>
+        <v>195</v>
       </c>
       <c r="L6">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>5010</v>
+        <v>64</v>
       </c>
       <c r="O6">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>137</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -6139,16 +6196,16 @@
         <v>25000</v>
       </c>
       <c r="B7">
-        <v>5803</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>7030</v>
+        <v>0</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
@@ -6157,31 +6214,31 @@
         <v>0</v>
       </c>
       <c r="H7" s="11">
-        <v>5745</v>
+        <v>331</v>
       </c>
       <c r="I7" s="11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J7" s="11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>5872</v>
+        <v>156</v>
       </c>
       <c r="L7">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="M7">
-        <v>276</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>7905</v>
+        <v>757</v>
       </c>
       <c r="O7">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>245</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -6189,49 +6246,49 @@
         <v>30000</v>
       </c>
       <c r="B8">
-        <v>6761</v>
+        <v>192</v>
       </c>
       <c r="C8">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>6124</v>
+        <v>179</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="11">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H8" s="11">
-        <v>7763</v>
+        <v>144</v>
       </c>
       <c r="I8" s="11">
-        <v>183</v>
+        <v>4</v>
       </c>
       <c r="J8" s="11">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>5017</v>
+        <v>571</v>
       </c>
       <c r="L8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>8495</v>
+        <v>492</v>
       </c>
       <c r="O8">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -6239,49 +6296,49 @@
         <v>35000</v>
       </c>
       <c r="B9">
-        <v>5864</v>
+        <v>84</v>
       </c>
       <c r="C9">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>5171</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
       </c>
       <c r="G9" s="11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H9" s="11">
-        <v>7120</v>
+        <v>187</v>
       </c>
       <c r="I9" s="11">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="J9" s="11">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>5459</v>
+        <v>400</v>
       </c>
       <c r="L9">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N9">
-        <v>7024</v>
+        <v>260</v>
       </c>
       <c r="O9">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -6289,49 +6346,49 @@
         <v>40000</v>
       </c>
       <c r="B10">
-        <v>4503</v>
+        <v>615</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>6254</v>
+        <v>353</v>
       </c>
       <c r="F10" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G10" s="11">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="H10" s="11">
-        <v>3992</v>
+        <v>221</v>
       </c>
       <c r="I10" s="11">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="J10" s="11">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>6959</v>
+        <v>132</v>
       </c>
       <c r="L10">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>5302</v>
+        <v>234</v>
       </c>
       <c r="O10">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -6339,43 +6396,43 @@
         <v>45000</v>
       </c>
       <c r="B11">
-        <v>4965</v>
+        <v>166</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>5147</v>
+        <v>148</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
       </c>
       <c r="G11" s="11">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H11" s="11">
-        <v>5317</v>
+        <v>203</v>
       </c>
       <c r="I11" s="11">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="J11" s="11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>7265</v>
+        <v>383</v>
       </c>
       <c r="L11">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>5305</v>
+        <v>387</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -6389,43 +6446,43 @@
         <v>50000</v>
       </c>
       <c r="B12">
-        <v>7251</v>
+        <v>488</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>6500</v>
+        <v>577</v>
       </c>
       <c r="F12" s="5">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G12" s="11">
         <v>0</v>
       </c>
       <c r="H12" s="11">
-        <v>5505</v>
+        <v>122</v>
       </c>
       <c r="I12" s="11">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="J12" s="11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>6836</v>
+        <v>489</v>
       </c>
       <c r="L12">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>8144</v>
+        <v>711</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -6439,16 +6496,16 @@
         <v>55000</v>
       </c>
       <c r="B13">
-        <v>5897</v>
+        <v>1250</v>
       </c>
       <c r="C13">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>6499</v>
+        <v>1347</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -6457,28 +6514,28 @@
         <v>0</v>
       </c>
       <c r="H13" s="11">
-        <v>7639</v>
+        <v>600</v>
       </c>
       <c r="I13" s="11">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="J13" s="11">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>5485</v>
+        <v>936</v>
       </c>
       <c r="L13">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>6364</v>
+        <v>786</v>
       </c>
       <c r="O13">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -6489,43 +6546,43 @@
         <v>60000</v>
       </c>
       <c r="B14">
-        <v>7291</v>
+        <v>996</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>7203</v>
+        <v>701</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
       </c>
       <c r="G14" s="11">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H14" s="11">
-        <v>7944</v>
+        <v>956</v>
       </c>
       <c r="I14" s="11">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="J14" s="11">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>5644</v>
+        <v>955</v>
       </c>
       <c r="L14">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>5694</v>
+        <v>868</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -6539,43 +6596,43 @@
         <v>65000</v>
       </c>
       <c r="B15">
-        <v>6941</v>
+        <v>395</v>
       </c>
       <c r="C15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>4688</v>
+        <v>519</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
       </c>
       <c r="G15" s="11">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H15" s="11">
-        <v>8268</v>
+        <v>1297</v>
       </c>
       <c r="I15" s="11">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="J15" s="11">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>5409</v>
+        <v>1101</v>
       </c>
       <c r="L15">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>6043</v>
+        <v>908</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -6589,16 +6646,16 @@
         <v>70000</v>
       </c>
       <c r="B16">
-        <v>8642</v>
+        <v>948</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>8045</v>
+        <v>604</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -6607,25 +6664,25 @@
         <v>0</v>
       </c>
       <c r="H16" s="11">
-        <v>7053</v>
+        <v>633</v>
       </c>
       <c r="I16" s="11">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="J16" s="11">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>4299</v>
+        <v>740</v>
       </c>
       <c r="L16">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>4748</v>
+        <v>934</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -6639,7 +6696,7 @@
         <v>75000</v>
       </c>
       <c r="B17">
-        <v>7034</v>
+        <v>161</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -6648,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>7948</v>
+        <v>859</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -6657,25 +6714,25 @@
         <v>0</v>
       </c>
       <c r="H17" s="11">
-        <v>7351</v>
+        <v>961</v>
       </c>
       <c r="I17" s="11">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="J17" s="11">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>3828</v>
+        <v>1297</v>
       </c>
       <c r="L17">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>4701</v>
+        <v>711</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -6689,16 +6746,16 @@
         <v>80000</v>
       </c>
       <c r="B18">
-        <v>7307</v>
+        <v>1199</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>5353</v>
+        <v>415</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
@@ -6707,10 +6764,10 @@
         <v>0</v>
       </c>
       <c r="H18" s="11">
-        <v>6175</v>
+        <v>622</v>
       </c>
       <c r="I18" s="11">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="J18" s="11">
         <v>0</v>
@@ -6721,28 +6778,28 @@
         <v>85000</v>
       </c>
       <c r="B19">
-        <v>4457</v>
+        <v>681</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>6345</v>
+        <v>748</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
       </c>
       <c r="G19" s="11">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H19" s="11">
-        <v>7826</v>
+        <v>166</v>
       </c>
       <c r="I19" s="11">
-        <v>116</v>
+        <v>4</v>
       </c>
       <c r="J19" s="11">
         <v>0</v>
@@ -6753,7 +6810,7 @@
         <v>90000</v>
       </c>
       <c r="B20">
-        <v>1450</v>
+        <v>991</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -6762,7 +6819,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>2263</v>
+        <v>781</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -6771,10 +6828,10 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>3675</v>
+        <v>759</v>
       </c>
       <c r="I20">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="J20" s="11">
         <v>0</v>
@@ -6784,15 +6841,33 @@
       <c r="A21" s="10">
         <v>95000</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="B21" s="1">
+        <v>873</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1104</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>914</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -6806,63 +6881,63 @@
       </c>
       <c r="B22">
         <f t="shared" ref="B22:P22" si="0">SUM(B3:B21)</f>
-        <v>108640</v>
+        <v>9840</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>347</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>60</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>110252</v>
+        <v>9244</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>54</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>117180</v>
+        <v>8765</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>1912</v>
+        <v>70</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>85172</v>
+        <v>8936</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>1542</v>
+        <v>23</v>
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>1313</v>
+        <v>57</v>
       </c>
       <c r="N22">
         <f t="shared" si="0"/>
-        <v>87933</v>
+        <v>7250</v>
       </c>
       <c r="O22">
         <f t="shared" si="0"/>
-        <v>997</v>
+        <v>0</v>
       </c>
       <c r="P22">
         <f t="shared" si="0"/>
-        <v>1033</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>